<commit_message>
de Assis 2011 results
</commit_message>
<xml_diff>
--- a/matrix_progress.xlsx
+++ b/matrix_progress.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="67">
   <si>
     <t>Aguado2009</t>
   </si>
@@ -623,7 +623,7 @@
   <dimension ref="A1:K35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" activeCellId="1" sqref="K6 K5"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -812,8 +812,11 @@
       <c r="I6" s="1">
         <v>1</v>
       </c>
-      <c r="J6" s="1" t="s">
-        <v>65</v>
+      <c r="J6" s="1">
+        <v>1</v>
+      </c>
+      <c r="K6" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
@@ -835,8 +838,11 @@
       <c r="H7" s="1">
         <v>1</v>
       </c>
-      <c r="I7" s="1">
-        <v>1</v>
+      <c r="I7" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
@@ -858,8 +864,8 @@
       <c r="H8" s="1">
         <v>1</v>
       </c>
-      <c r="I8" s="1" t="s">
-        <v>65</v>
+      <c r="I8" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
@@ -881,8 +887,8 @@
       <c r="H9" s="1">
         <v>1</v>
       </c>
-      <c r="I9" s="1" t="s">
-        <v>65</v>
+      <c r="I9" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Rousset 2004 complete & plotted
</commit_message>
<xml_diff>
--- a/matrix_progress.xlsx
+++ b/matrix_progress.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="67">
   <si>
     <t>Aguado2009</t>
   </si>
@@ -838,11 +838,14 @@
       <c r="H7" s="1">
         <v>1</v>
       </c>
-      <c r="I7" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>65</v>
+      <c r="I7" s="1">
+        <v>1</v>
+      </c>
+      <c r="J7" s="1">
+        <v>1</v>
+      </c>
+      <c r="K7" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
@@ -867,6 +870,9 @@
       <c r="I8" s="1">
         <v>1</v>
       </c>
+      <c r="J8" s="1" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
@@ -978,6 +984,9 @@
       </c>
       <c r="E13" s="1">
         <v>58</v>
+      </c>
+      <c r="H13" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
New approach to plotting; clear the decks
</commit_message>
<xml_diff>
--- a/matrix_progress.xlsx
+++ b/matrix_progress.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="70">
   <si>
     <t>Aguado2009</t>
   </si>
@@ -138,9 +138,6 @@
   </si>
   <si>
     <t>rRuns</t>
-  </si>
-  <si>
-    <t>pdfOut</t>
   </si>
   <si>
     <t>Conrad2008 [nee Wiens2010]</t>
@@ -290,14 +287,14 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="7"/>
+          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
+          <bgColor theme="7"/>
         </patternFill>
       </fill>
     </dxf>
@@ -611,10 +608,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A103D6C0-D7FF-4DC9-A848-61273A1C93D6}">
-  <dimension ref="A1:L35"/>
+  <dimension ref="A1:K35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -633,7 +630,7 @@
     <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>34</v>
       </c>
@@ -641,10 +638,10 @@
         <v>30</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>31</v>
@@ -665,13 +662,10 @@
         <v>37</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
@@ -691,10 +685,10 @@
         <v>5.7</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -722,19 +716,16 @@
       <c r="J3" s="1">
         <v>1</v>
       </c>
-      <c r="K3" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D4" s="1">
         <v>23</v>
@@ -757,16 +748,13 @@
       <c r="J4" s="1">
         <v>1</v>
       </c>
-      <c r="K4" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D5" s="1">
         <v>23</v>
@@ -783,22 +771,16 @@
       <c r="J5" s="1">
         <v>1</v>
       </c>
-      <c r="K5" s="1">
-        <v>1</v>
-      </c>
-      <c r="L5" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D6" s="1">
         <v>33</v>
@@ -815,19 +797,16 @@
       <c r="J6" s="1">
         <v>1</v>
       </c>
-      <c r="K6" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D7" s="1">
         <v>34</v>
@@ -844,19 +823,16 @@
       <c r="J7" s="1">
         <v>1</v>
       </c>
-      <c r="K7" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D8" s="1">
         <v>35</v>
@@ -873,19 +849,16 @@
       <c r="J8" s="1">
         <v>1</v>
       </c>
-      <c r="K8" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>62</v>
       </c>
       <c r="D9" s="1">
         <v>36</v>
@@ -902,11 +875,8 @@
       <c r="J9" s="1">
         <v>1</v>
       </c>
-      <c r="K9" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>28</v>
       </c>
@@ -934,19 +904,16 @@
       <c r="J10" s="1">
         <v>1</v>
       </c>
-      <c r="K10" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>64</v>
       </c>
       <c r="D11" s="1">
         <v>40</v>
@@ -963,11 +930,8 @@
       <c r="J11" s="1">
         <v>1</v>
       </c>
-      <c r="K11" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
@@ -995,16 +959,13 @@
       <c r="J12" s="1">
         <v>1</v>
       </c>
-      <c r="K12" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D13" s="1">
         <v>52</v>
@@ -1022,7 +983,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>9</v>
       </c>
@@ -1050,19 +1011,16 @@
       <c r="J14" s="1">
         <v>1</v>
       </c>
-      <c r="K14" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D15" s="1">
         <v>55</v>
@@ -1080,7 +1038,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
@@ -1106,9 +1064,6 @@
         <v>1</v>
       </c>
       <c r="J16" s="1">
-        <v>1</v>
-      </c>
-      <c r="K16" s="1">
         <v>1</v>
       </c>
     </row>
@@ -1143,13 +1098,13 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>68</v>
       </c>
       <c r="D18" s="1">
         <v>59</v>
@@ -1195,13 +1150,13 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D20" s="1">
         <v>62</v>
@@ -1213,6 +1168,9 @@
         <v>1</v>
       </c>
       <c r="I20" s="1">
+        <v>1</v>
+      </c>
+      <c r="J20" s="1">
         <v>1</v>
       </c>
     </row>
@@ -1241,16 +1199,16 @@
       <c r="I21" s="1">
         <v>1</v>
       </c>
-      <c r="J21" s="1" t="s">
-        <v>65</v>
+      <c r="J21" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D22" s="1">
         <v>63</v>
@@ -1267,7 +1225,7 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>25</v>
@@ -1290,16 +1248,19 @@
       <c r="I23" s="1">
         <v>1</v>
       </c>
+      <c r="J23" s="1" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D24" s="1">
         <v>67</v>
@@ -1311,6 +1272,12 @@
         <v>1</v>
       </c>
       <c r="I24" s="1">
+        <v>1</v>
+      </c>
+      <c r="J24" s="1">
+        <v>1</v>
+      </c>
+      <c r="K24" s="1">
         <v>1</v>
       </c>
     </row>
@@ -1342,9 +1309,6 @@
       <c r="J25" s="1">
         <v>1</v>
       </c>
-      <c r="K25" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
@@ -1426,9 +1390,6 @@
       <c r="J28" s="1">
         <v>1</v>
       </c>
-      <c r="K28" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
@@ -1458,7 +1419,7 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>1</v>
@@ -1583,11 +1544,11 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:L35">
+  <sortState ref="A2:K35">
     <sortCondition ref="D2:D35"/>
   </sortState>
-  <conditionalFormatting sqref="H2:K35 L3:L35">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
+  <conditionalFormatting sqref="H2:J35 K3:K35">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1608,7 +1569,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>H2:K35 L3:L35</xm:sqref>
+          <xm:sqref>H2:J35 K3:K35</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
Getting there; needs updataing
</commit_message>
<xml_diff>
--- a/matrix_progress.xlsx
+++ b/matrix_progress.xlsx
@@ -611,7 +611,7 @@
   <dimension ref="A1:K35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -667,45 +667,45 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>56</v>
       </c>
       <c r="D2" s="1">
-        <v>19</v>
+        <v>62</v>
       </c>
       <c r="E2" s="1">
-        <v>119</v>
-      </c>
-      <c r="F2" s="1">
-        <v>26.1</v>
-      </c>
-      <c r="G2" s="1">
-        <v>5.7</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>64</v>
+        <v>242</v>
+      </c>
+      <c r="H2" s="1">
+        <v>1</v>
+      </c>
+      <c r="I2" s="1">
+        <v>1</v>
+      </c>
+      <c r="J2" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>42</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>56</v>
       </c>
       <c r="D3" s="1">
-        <v>23</v>
+        <v>67</v>
       </c>
       <c r="E3" s="1">
-        <v>126</v>
-      </c>
-      <c r="F3" s="1">
-        <v>31.7</v>
-      </c>
-      <c r="G3" s="1">
-        <v>3.9</v>
+        <v>135</v>
       </c>
       <c r="H3" s="1">
         <v>1</v>
@@ -714,30 +714,27 @@
         <v>1</v>
       </c>
       <c r="J3" s="1">
+        <v>1</v>
+      </c>
+      <c r="K3" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>54</v>
+        <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D4" s="1">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="E4" s="1">
-        <v>57</v>
-      </c>
-      <c r="F4" s="1">
-        <v>43.9</v>
-      </c>
-      <c r="G4" s="1">
-        <v>20.9</v>
+        <v>50</v>
       </c>
       <c r="H4" s="1">
         <v>1</v>
@@ -751,16 +748,19 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>53</v>
+        <v>62</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="D5" s="1">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="E5" s="1">
-        <v>109</v>
+        <v>150</v>
       </c>
       <c r="H5" s="1">
         <v>1</v>
@@ -774,7 +774,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>43</v>
+        <v>65</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>1</v>
@@ -783,10 +783,10 @@
         <v>56</v>
       </c>
       <c r="D6" s="1">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E6" s="1">
-        <v>50</v>
+        <v>107</v>
       </c>
       <c r="H6" s="1">
         <v>1</v>
@@ -800,19 +800,19 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="D7" s="1">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E7" s="1">
-        <v>107</v>
+        <v>52</v>
       </c>
       <c r="H7" s="1">
         <v>1</v>
@@ -826,19 +826,16 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D8" s="1">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="E8" s="1">
-        <v>50</v>
+        <v>109</v>
       </c>
       <c r="H8" s="1">
         <v>1</v>
@@ -852,19 +849,16 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="D9" s="1">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="E9" s="1">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="H9" s="1">
         <v>1</v>
@@ -878,22 +872,19 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>5</v>
+        <v>66</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="D10" s="1">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="E10" s="1">
-        <v>105</v>
-      </c>
-      <c r="F10" s="1">
-        <v>20</v>
-      </c>
-      <c r="G10" s="1">
-        <v>3.7</v>
+        <v>202</v>
       </c>
       <c r="H10" s="1">
         <v>1</v>
@@ -907,16 +898,13 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C11" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D11" s="1">
         <v>63</v>
-      </c>
-      <c r="D11" s="1">
-        <v>40</v>
       </c>
       <c r="E11" s="1">
         <v>150</v>
@@ -927,28 +915,22 @@
       <c r="I11" s="1">
         <v>1</v>
       </c>
-      <c r="J11" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>14</v>
+        <v>55</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>58</v>
       </c>
       <c r="D12" s="1">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="E12" s="1">
-        <v>137</v>
-      </c>
-      <c r="F12" s="1">
-        <v>43.8</v>
-      </c>
-      <c r="G12" s="1">
-        <v>9.6</v>
+        <v>88</v>
       </c>
       <c r="H12" s="1">
         <v>1</v>
@@ -962,16 +944,22 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>47</v>
+        <v>0</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>52</v>
+        <v>1</v>
       </c>
       <c r="D13" s="1">
-        <v>52</v>
+        <v>76</v>
       </c>
       <c r="E13" s="1">
-        <v>58</v>
+        <v>107</v>
+      </c>
+      <c r="F13" s="1">
+        <v>40.200000000000003</v>
+      </c>
+      <c r="G13" s="1">
+        <v>5</v>
       </c>
       <c r="H13" s="1">
         <v>1</v>
@@ -985,22 +973,19 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>9</v>
+        <v>40</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>5</v>
+        <v>59</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>58</v>
       </c>
       <c r="D14" s="1">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="E14" s="1">
-        <v>131</v>
-      </c>
-      <c r="F14" s="1">
-        <v>31.3</v>
-      </c>
-      <c r="G14" s="1">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="H14" s="1">
         <v>1</v>
@@ -1014,19 +999,22 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>50</v>
+        <v>2</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>58</v>
+        <v>3</v>
       </c>
       <c r="D15" s="1">
-        <v>55</v>
+        <v>23</v>
       </c>
       <c r="E15" s="1">
-        <v>88</v>
+        <v>126</v>
+      </c>
+      <c r="F15" s="1">
+        <v>31.7</v>
+      </c>
+      <c r="G15" s="1">
+        <v>3.9</v>
       </c>
       <c r="H15" s="1">
         <v>1</v>
@@ -1040,77 +1028,62 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D16" s="1">
-        <v>56</v>
+        <v>205</v>
       </c>
       <c r="E16" s="1">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F16" s="1">
-        <v>63.5</v>
+        <v>35.200000000000003</v>
       </c>
       <c r="G16" s="1">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="H16" s="1">
-        <v>1</v>
-      </c>
-      <c r="I16" s="1">
-        <v>1</v>
-      </c>
-      <c r="J16" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+        <v>8.3000000000000007</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D17" s="1">
-        <v>58</v>
+        <v>818</v>
       </c>
       <c r="E17" s="1">
-        <v>317</v>
+        <v>417</v>
       </c>
       <c r="F17" s="1">
-        <v>2.8</v>
+        <v>81.5</v>
       </c>
       <c r="G17" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="H17" s="1">
-        <v>1</v>
-      </c>
-      <c r="I17" s="1">
-        <v>1</v>
-      </c>
-      <c r="J17" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+        <v>21.1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>67</v>
+        <v>25</v>
       </c>
       <c r="D18" s="1">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="E18" s="1">
-        <v>202</v>
+        <v>363</v>
+      </c>
+      <c r="F18" s="1">
+        <v>41.9</v>
+      </c>
+      <c r="G18" s="1">
+        <v>7.7</v>
       </c>
       <c r="H18" s="1">
         <v>1</v>
@@ -1118,28 +1091,28 @@
       <c r="I18" s="1">
         <v>1</v>
       </c>
-      <c r="J18" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J18" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="D19" s="1">
-        <v>61</v>
+        <v>88</v>
       </c>
       <c r="E19" s="1">
-        <v>165</v>
+        <v>220</v>
       </c>
       <c r="F19" s="1">
-        <v>43</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="G19" s="1">
-        <v>11.1</v>
+        <v>1.6</v>
       </c>
       <c r="H19" s="1">
         <v>1</v>
@@ -1148,21 +1121,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>41</v>
+        <v>9</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>56</v>
+        <v>5</v>
       </c>
       <c r="D20" s="1">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="E20" s="1">
-        <v>242</v>
+        <v>131</v>
+      </c>
+      <c r="F20" s="1">
+        <v>31.3</v>
+      </c>
+      <c r="G20" s="1">
+        <v>10</v>
       </c>
       <c r="H20" s="1">
         <v>1</v>
@@ -1174,378 +1150,402 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D21" s="1">
+        <v>68</v>
+      </c>
+      <c r="E21" s="1">
+        <v>186</v>
+      </c>
+      <c r="F21" s="1">
+        <v>46.8</v>
+      </c>
+      <c r="G21" s="1">
+        <v>2</v>
+      </c>
+      <c r="H21" s="1">
+        <v>1</v>
+      </c>
+      <c r="I21" s="1">
+        <v>1</v>
+      </c>
+      <c r="J21" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" s="1">
+        <v>78</v>
+      </c>
+      <c r="E22" s="1">
+        <v>236</v>
+      </c>
+      <c r="F22" s="1">
+        <v>74.2</v>
+      </c>
+      <c r="G22" s="1">
+        <v>17.3</v>
+      </c>
+      <c r="H22" s="1">
+        <v>1</v>
+      </c>
+      <c r="I22" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" s="1">
+        <v>43</v>
+      </c>
+      <c r="E23" s="1">
+        <v>137</v>
+      </c>
+      <c r="F23" s="1">
+        <v>43.8</v>
+      </c>
+      <c r="G23" s="1">
+        <v>9.6</v>
+      </c>
+      <c r="H23" s="1">
+        <v>1</v>
+      </c>
+      <c r="I23" s="1">
+        <v>1</v>
+      </c>
+      <c r="J23" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" s="1">
+        <v>68</v>
+      </c>
+      <c r="E24" s="1">
+        <v>308</v>
+      </c>
+      <c r="F24" s="1">
+        <v>31.5</v>
+      </c>
+      <c r="G24" s="1">
+        <v>6.4</v>
+      </c>
+      <c r="H24" s="1">
+        <v>1</v>
+      </c>
+      <c r="I24" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" s="1">
+        <v>56</v>
+      </c>
+      <c r="E25" s="1">
+        <v>104</v>
+      </c>
+      <c r="F25" s="1">
+        <v>63.5</v>
+      </c>
+      <c r="G25" s="1">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="H25" s="1">
+        <v>1</v>
+      </c>
+      <c r="I25" s="1">
+        <v>1</v>
+      </c>
+      <c r="J25" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D26" s="1">
+        <v>19</v>
+      </c>
+      <c r="E26" s="1">
+        <v>119</v>
+      </c>
+      <c r="F26" s="1">
+        <v>26.1</v>
+      </c>
+      <c r="G26" s="1">
+        <v>5.7</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D27" s="1">
         <v>63</v>
       </c>
-      <c r="E21" s="1">
+      <c r="E27" s="1">
         <v>317</v>
       </c>
-      <c r="F21" s="1">
+      <c r="F27" s="1">
         <v>44.5</v>
       </c>
-      <c r="G21" s="1">
+      <c r="G27" s="1">
         <v>5.4</v>
       </c>
-      <c r="H21" s="1">
-        <v>1</v>
-      </c>
-      <c r="I21" s="1">
-        <v>1</v>
-      </c>
-      <c r="J21" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D22" s="1">
-        <v>63</v>
-      </c>
-      <c r="E22" s="1">
-        <v>150</v>
-      </c>
-      <c r="H22" s="1">
-        <v>1</v>
-      </c>
-      <c r="I22" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D23" s="1">
-        <v>64</v>
-      </c>
-      <c r="E23" s="1">
-        <v>363</v>
-      </c>
-      <c r="F23" s="1">
-        <v>41.9</v>
-      </c>
-      <c r="G23" s="1">
-        <v>7.7</v>
-      </c>
-      <c r="H23" s="1">
-        <v>1</v>
-      </c>
-      <c r="I23" s="1">
-        <v>1</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D24" s="1">
-        <v>67</v>
-      </c>
-      <c r="E24" s="1">
-        <v>135</v>
-      </c>
-      <c r="H24" s="1">
-        <v>1</v>
-      </c>
-      <c r="I24" s="1">
-        <v>1</v>
-      </c>
-      <c r="J24" s="1">
-        <v>1</v>
-      </c>
-      <c r="K24" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B25" s="1" t="s">
+      <c r="H27" s="1">
+        <v>1</v>
+      </c>
+      <c r="I27" s="1">
+        <v>1</v>
+      </c>
+      <c r="J27" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D25" s="1">
-        <v>68</v>
-      </c>
-      <c r="E25" s="1">
-        <v>186</v>
-      </c>
-      <c r="F25" s="1">
-        <v>46.8</v>
-      </c>
-      <c r="G25" s="1">
-        <v>2</v>
-      </c>
-      <c r="H25" s="1">
-        <v>1</v>
-      </c>
-      <c r="I25" s="1">
-        <v>1</v>
-      </c>
-      <c r="J25" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B26" s="1" t="s">
+      <c r="D28" s="1">
+        <v>58</v>
+      </c>
+      <c r="E28" s="1">
+        <v>317</v>
+      </c>
+      <c r="F28" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="G28" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="H28" s="1">
+        <v>1</v>
+      </c>
+      <c r="I28" s="1">
+        <v>1</v>
+      </c>
+      <c r="J28" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D26" s="1">
-        <v>68</v>
-      </c>
-      <c r="E26" s="1">
-        <v>308</v>
-      </c>
-      <c r="F26" s="1">
-        <v>31.5</v>
-      </c>
-      <c r="G26" s="1">
-        <v>6.4</v>
-      </c>
-      <c r="H26" s="1">
-        <v>1</v>
-      </c>
-      <c r="I26" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
+      <c r="D29" s="1">
+        <v>105</v>
+      </c>
+      <c r="E29" s="1">
+        <v>392</v>
+      </c>
+      <c r="F29" s="1">
+        <v>100</v>
+      </c>
+      <c r="G29" s="1">
+        <v>20.100000000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D30" s="1">
+        <v>177</v>
+      </c>
+      <c r="E30" s="1">
+        <v>237</v>
+      </c>
+      <c r="F30" s="1">
+        <v>81.900000000000006</v>
+      </c>
+      <c r="G30" s="1">
+        <v>26.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D31" s="1">
+        <v>23</v>
+      </c>
+      <c r="E31" s="1">
+        <v>57</v>
+      </c>
+      <c r="F31" s="1">
+        <v>43.9</v>
+      </c>
+      <c r="G31" s="1">
+        <v>20.9</v>
+      </c>
+      <c r="H31" s="1">
+        <v>1</v>
+      </c>
+      <c r="I31" s="1">
+        <v>1</v>
+      </c>
+      <c r="J31" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D32" s="1">
+        <v>61</v>
+      </c>
+      <c r="E32" s="1">
+        <v>165</v>
+      </c>
+      <c r="F32" s="1">
+        <v>43</v>
+      </c>
+      <c r="G32" s="1">
+        <v>11.1</v>
+      </c>
+      <c r="H32" s="1">
+        <v>1</v>
+      </c>
+      <c r="I32" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D33" s="1">
+        <v>37</v>
+      </c>
+      <c r="E33" s="1">
+        <v>105</v>
+      </c>
+      <c r="F33" s="1">
+        <v>20</v>
+      </c>
+      <c r="G33" s="1">
+        <v>3.7</v>
+      </c>
+      <c r="H33" s="1">
+        <v>1</v>
+      </c>
+      <c r="I33" s="1">
+        <v>1</v>
+      </c>
+      <c r="J33" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D34" s="1">
+        <v>74</v>
+      </c>
+      <c r="E34" s="1">
+        <v>213</v>
+      </c>
+      <c r="H34" s="1">
+        <v>1</v>
+      </c>
+      <c r="I34" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B35" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D27" s="1">
+      <c r="D35" s="1">
         <v>75</v>
       </c>
-      <c r="E27" s="1">
+      <c r="E35" s="1">
         <v>253</v>
       </c>
-      <c r="F27" s="1">
+      <c r="F35" s="1">
         <v>70.8</v>
       </c>
-      <c r="G27" s="1">
+      <c r="G35" s="1">
         <v>19.3</v>
       </c>
-      <c r="H27" s="1">
-        <v>1</v>
-      </c>
-      <c r="I27" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D28" s="1">
-        <v>76</v>
-      </c>
-      <c r="E28" s="1">
-        <v>107</v>
-      </c>
-      <c r="F28" s="1">
-        <v>40.200000000000003</v>
-      </c>
-      <c r="G28" s="1">
-        <v>5</v>
-      </c>
-      <c r="H28" s="1">
-        <v>1</v>
-      </c>
-      <c r="I28" s="1">
-        <v>1</v>
-      </c>
-      <c r="J28" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D29" s="1">
-        <v>78</v>
-      </c>
-      <c r="E29" s="1">
-        <v>236</v>
-      </c>
-      <c r="F29" s="1">
-        <v>74.2</v>
-      </c>
-      <c r="G29" s="1">
-        <v>17.3</v>
-      </c>
-      <c r="H29" s="1">
-        <v>1</v>
-      </c>
-      <c r="I29" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D30" s="1">
-        <v>74</v>
-      </c>
-      <c r="E30" s="1">
-        <v>213</v>
-      </c>
-      <c r="H30" s="1">
-        <v>1</v>
-      </c>
-      <c r="I30" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D31" s="1">
-        <v>88</v>
-      </c>
-      <c r="E31" s="1">
-        <v>220</v>
-      </c>
-      <c r="F31" s="1">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="G31" s="1">
-        <v>1.6</v>
-      </c>
-      <c r="H31" s="1">
-        <v>1</v>
-      </c>
-      <c r="I31" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D32" s="1">
-        <v>105</v>
-      </c>
-      <c r="E32" s="1">
-        <v>392</v>
-      </c>
-      <c r="F32" s="1">
-        <v>100</v>
-      </c>
-      <c r="G32" s="1">
-        <v>20.100000000000001</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D33" s="1">
-        <v>177</v>
-      </c>
-      <c r="E33" s="1">
-        <v>237</v>
-      </c>
-      <c r="F33" s="1">
-        <v>81.900000000000006</v>
-      </c>
-      <c r="G33" s="1">
-        <v>26.5</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D34" s="1">
-        <v>205</v>
-      </c>
-      <c r="E34" s="1">
-        <v>105</v>
-      </c>
-      <c r="F34" s="1">
-        <v>35.200000000000003</v>
-      </c>
-      <c r="G34" s="1">
-        <v>8.3000000000000007</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D35" s="1">
-        <v>818</v>
-      </c>
-      <c r="E35" s="1">
-        <v>417</v>
-      </c>
-      <c r="F35" s="1">
-        <v>81.5</v>
-      </c>
-      <c r="G35" s="1">
-        <v>21.1</v>
+      <c r="H35" s="1">
+        <v>1</v>
+      </c>
+      <c r="I35" s="1">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <sortState ref="A2:K35">
-    <sortCondition ref="D2:D35"/>
+    <sortCondition ref="A2:A35"/>
   </sortState>
   <conditionalFormatting sqref="H2:J35 K3:K35">
     <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">

</xml_diff>